<commit_message>
Updated Excel to YAML utility for dynamic handling of columns
</commit_message>
<xml_diff>
--- a/input/Semantic_design_template.xlsx
+++ b/input/Semantic_design_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bayergroup-my.sharepoint.com/personal/ankit_kumar8_ext_bayer_com/Documents/downloads1/utilityUS/excel-to-yaml/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="13_ncr:1_{A6554839-2BA0-4F6B-B9B7-B2EA66B5D24C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A077A78-EE20-490C-8354-4399B0B4BCEA}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="13_ncr:1_{A6554839-2BA0-4F6B-B9B7-B2EA66B5D24C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{205C708C-9887-4BD8-8A78-155056DD1610}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{104D53FC-4049-A745-9D84-591BF0B6341D}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
   <si>
     <t>table</t>
   </si>
@@ -141,6 +141,15 @@
   </si>
   <si>
     <t>sum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 things which are in sample excel but not in here -&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. dim_measure_flag </t>
+  </si>
+  <si>
+    <t>2. views_col_names</t>
   </si>
 </sst>
 </file>
@@ -168,7 +177,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,6 +187,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -194,14 +209,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,15 +556,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91C9AE3B-DA75-D04F-9B0C-1D6B12D9A39D}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5" bestFit="1" customWidth="1"/>
@@ -556,16 +576,16 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" t="s">
@@ -576,20 +596,35 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="5" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -605,7 +640,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75"/>
@@ -621,16 +656,16 @@
       <c r="A1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -641,13 +676,13 @@
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="5" t="s">
         <v>18</v>
       </c>
     </row>
@@ -664,7 +699,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75"/>
@@ -698,22 +733,22 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="113.1" customHeight="1">
-      <c r="A2" t="s">
+      <c r="A2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E2" t="b">
+      <c r="E2" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="5" t="s">
         <v>27</v>
       </c>
     </row>
@@ -730,12 +765,12 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
@@ -760,19 +795,19 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>